<commit_message>
Added ability to make a move and flip relevant peices
</commit_message>
<xml_diff>
--- a/ReversiKata01/Book1.xlsx
+++ b/ReversiKata01/Book1.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\alan\repos\NewRepo\ReversiKata\ReversiKata01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanv\source\repos\ReversiKata\ReversiKata01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D942B65-0F8E-4FF3-89EF-C34559D718AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E920421-E3E7-4844-A0DA-25B700DF089B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{486067F7-353F-43AD-87A8-01116A4CD49D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" activeTab="2" xr2:uid="{486067F7-353F-43AD-87A8-01116A4CD49D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="4">
   <si>
     <t>B</t>
   </si>
@@ -40,6 +43,9 @@
   </si>
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -90,10 +96,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -412,18 +421,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5464D941-5696-4E11-A275-8616510D2D30}">
   <dimension ref="A2:Q10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="1" max="9" width="2.81640625" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
     <col min="11" max="17" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>0</v>
       </c>
@@ -449,7 +458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -470,7 +479,7 @@
         <v/>
       </c>
       <c r="M3" s="1" t="str">
-        <f t="shared" ref="M3:M10" si="2">IF(E3="o", "(" &amp; E$2 &amp; "," &amp; $A3 &amp; ")", "")</f>
+        <f t="shared" ref="M3:M4" si="2">IF(E3="o", "(" &amp; E$2 &amp; "," &amp; $A3 &amp; ")", "")</f>
         <v/>
       </c>
       <c r="N3" s="1" t="str">
@@ -490,7 +499,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -531,14 +540,16 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
@@ -555,7 +566,7 @@
       </c>
       <c r="M5" s="1" t="str">
         <f>IF(E5="o", "(" &amp; E$2 &amp; "," &amp; $A5 &amp; ")", "")</f>
-        <v/>
+        <v>(3,2)</v>
       </c>
       <c r="N5" s="1" t="str">
         <f t="shared" si="3"/>
@@ -574,13 +585,15 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
@@ -598,7 +611,7 @@
       </c>
       <c r="L6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>(2,3)</v>
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" ref="M6:M10" si="7">IF(E6="o", "(" &amp; E$2 &amp; "," &amp; $A6 &amp; ")", "")</f>
@@ -621,7 +634,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -668,7 +681,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -711,7 +724,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -752,7 +765,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -797,4 +810,1020 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E8439E-6BB0-4CC5-8487-46CB019CDEE0}">
+  <dimension ref="A2:Q10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="9" width="2.81640625" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
+    <col min="11" max="17" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:Q10" si="0">IF(C3="o", "(" &amp; C$2 &amp; "," &amp; $A3 &amp; ")", "")</f>
+        <v/>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f>IF(E5="o", "(" &amp; E$2 &amp; "," &amp; $A5 &amp; ")", "")</f>
+        <v/>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7564A42-D314-4087-845E-9D97F50EFF0F}">
+  <dimension ref="A2:Q10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="9" width="2.81640625" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
+    <col min="11" max="17" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:Q10" si="0">IF(C3="o", "(" &amp; C$2 &amp; "," &amp; $A3 &amp; ")", "")</f>
+        <v/>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f>IF(E5="o", "(" &amp; E$2 &amp; "," &amp; $A5 &amp; ")", "")</f>
+        <v/>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC96129-24E2-46BE-82D9-050733CEF831}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change to game tracking spreadsheet
</commit_message>
<xml_diff>
--- a/ReversiKata01/Book1.xlsx
+++ b/ReversiKata01/Book1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanv\source\repos\ReversiKata\ReversiKata01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E920421-E3E7-4844-A0DA-25B700DF089B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EEC92B-2D23-4540-80CC-B0F9C9C199D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" activeTab="2" xr2:uid="{486067F7-353F-43AD-87A8-01116A4CD49D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" activeTab="3" xr2:uid="{486067F7-353F-43AD-87A8-01116A4CD49D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1 (3)" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1 (4)" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="4">
   <si>
     <t>B</t>
   </si>
@@ -1317,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7564A42-D314-4087-845E-9D97F50EFF0F}">
   <dimension ref="A2:Q10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1817,6 +1818,507 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F0EDCA-A3C5-443F-8ACF-DDA38B19DC05}">
+  <dimension ref="A2:Q10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="9" width="2.81640625" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
+    <col min="11" max="17" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:Q10" si="0">IF(C3="o", "(" &amp; C$2 &amp; "," &amp; $A3 &amp; ")", "")</f>
+        <v/>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f>IF(E5="o", "(" &amp; E$2 &amp; "," &amp; $A5 &amp; ")", "")</f>
+        <v/>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC96129-24E2-46BE-82D9-050733CEF831}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>